<commit_message>
integración con python y fix ranking
</commit_message>
<xml_diff>
--- a/datos/geo/estaciones.xlsx
+++ b/datos/geo/estaciones.xlsx
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1628786984</v>
+        <v>1629830948</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -527,10 +527,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
         <v>-32.95421439665977</v>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1628786975</v>
+        <v>1629830951</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -571,10 +571,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
         <v>-32.95666307690848</v>
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1628786997</v>
+        <v>1629830955</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -615,10 +615,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K4" t="n">
         <v>-32.95812144981906</v>
@@ -650,19 +650,19 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1628786988</v>
+        <v>1629830943</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
+        <v>9</v>
+      </c>
+      <c r="J5" t="n">
         <v>11</v>
-      </c>
-      <c r="J5" t="n">
-        <v>9</v>
       </c>
       <c r="K5" t="n">
         <v>-32.95921521370776</v>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1628786971</v>
+        <v>1629830941</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -703,10 +703,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K6" t="n">
         <v>-32.96736625395059</v>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1628786990</v>
+        <v>1629830945</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -747,10 +747,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K7" t="n">
         <v>-32.96850040867347</v>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>1628786994</v>
+        <v>1629830935</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -791,10 +791,10 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" t="n">
         <v>-32.93944885753075</v>
@@ -826,19 +826,19 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1628786982</v>
+        <v>1629830944</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I9" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J9" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K9" t="n">
         <v>-32.9403492658816</v>
@@ -870,19 +870,19 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1628786997</v>
+        <v>1629830951</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K10" t="n">
         <v>-32.94573801821987</v>
@@ -914,7 +914,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1628786974</v>
+        <v>1629830937</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
@@ -958,7 +958,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1628786986</v>
+        <v>1629830952</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -967,10 +967,10 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
+        <v>9</v>
+      </c>
+      <c r="J12" t="n">
         <v>10</v>
-      </c>
-      <c r="J12" t="n">
-        <v>9</v>
       </c>
       <c r="K12" t="n">
         <v>-32.94402733877261</v>
@@ -1002,19 +1002,19 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1628786988</v>
+        <v>1629830931</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J13" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K13" t="n">
         <v>-32.94531035146112</v>
@@ -1046,13 +1046,13 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>1628786973</v>
+        <v>1629830942</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
         <v>18</v>
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1628786979</v>
+        <v>1629830942</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -1099,10 +1099,10 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J15" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K15" t="n">
         <v>-32.94882616098827</v>
@@ -1134,13 +1134,13 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1628786992</v>
+        <v>1629830937</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
         <v>18</v>
@@ -1178,7 +1178,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1628786977</v>
+        <v>1629830926</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
@@ -1187,10 +1187,10 @@
         <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="J17" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="K17" t="n">
         <v>-32.93659000025387</v>
@@ -1222,19 +1222,19 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1628786974</v>
+        <v>1629830947</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="J18" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K18" t="n">
         <v>-32.93587864817957</v>
@@ -1266,19 +1266,19 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1628786976</v>
+        <v>1629830946</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
+        <v>8</v>
+      </c>
+      <c r="J19" t="n">
         <v>11</v>
-      </c>
-      <c r="J19" t="n">
-        <v>8</v>
       </c>
       <c r="K19" t="n">
         <v>-32.94099755421734</v>
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1628786977</v>
+        <v>1629830942</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
@@ -1319,10 +1319,10 @@
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K20" t="n">
         <v>-32.95358421061909</v>
@@ -1354,19 +1354,19 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1628786975</v>
+        <v>1629830945</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J21" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
         <v>-32.95206724436681</v>
@@ -1398,7 +1398,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>1628786994</v>
+        <v>1629830941</v>
       </c>
       <c r="G22" t="b">
         <v>0</v>
@@ -1407,10 +1407,10 @@
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J22" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K22" t="n">
         <v>-32.96512040461018</v>
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1628786979</v>
+        <v>1629830946</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -1451,10 +1451,10 @@
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J23" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="K23" t="n">
         <v>-32.92663505330592</v>
@@ -1486,19 +1486,19 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>1628786989</v>
+        <v>1629830946</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J24" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="K24" t="n">
         <v>-32.93184904583995</v>
@@ -1530,19 +1530,19 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>1628786998</v>
+        <v>1629830942</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
       </c>
       <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>19</v>
+      </c>
+      <c r="J25" t="n">
         <v>1</v>
-      </c>
-      <c r="I25" t="n">
-        <v>16</v>
-      </c>
-      <c r="J25" t="n">
-        <v>4</v>
       </c>
       <c r="K25" t="n">
         <v>-32.94041229412281</v>
@@ -1574,19 +1574,19 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>1628787000</v>
+        <v>1629830939</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K26" t="n">
         <v>-32.96268096048085</v>
@@ -1618,19 +1618,19 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1628786988</v>
+        <v>1629830927</v>
       </c>
       <c r="G27" t="b">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J27" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K27" t="n">
         <v>-32.96806835144843</v>
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>1628786975</v>
+        <v>1629830936</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
@@ -1671,10 +1671,10 @@
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J28" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="K28" t="n">
         <v>-32.96399070730771</v>
@@ -1706,19 +1706,19 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>1628786995</v>
+        <v>1629830952</v>
       </c>
       <c r="G29" t="b">
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I29" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K29" t="n">
         <v>-32.95339515393067</v>
@@ -1750,19 +1750,19 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1628786980</v>
+        <v>1629830930</v>
       </c>
       <c r="G30" t="b">
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J30" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K30" t="n">
         <v>-32.93516278810112</v>
@@ -1794,19 +1794,19 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1628786979</v>
+        <v>1629830926</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J31" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K31" t="n">
         <v>-32.94162782998716</v>
@@ -1838,19 +1838,19 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>1628786976</v>
+        <v>1629830927</v>
       </c>
       <c r="G32" t="b">
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J32" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K32" t="n">
         <v>-32.95894064873677</v>
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1628786974</v>
+        <v>1629830939</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
@@ -1926,19 +1926,19 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>1628786998</v>
+        <v>1629830937</v>
       </c>
       <c r="G34" t="b">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K34" t="n">
         <v>-32.94575602519591</v>
@@ -1970,13 +1970,13 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1628786980</v>
+        <v>1629830937</v>
       </c>
       <c r="G35" t="b">
         <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I35" t="n">
         <v>12</v>
@@ -1988,7 +1988,7 @@
         <v>-32.9556277975818</v>
       </c>
       <c r="L35" t="n">
-        <v>-60.65117239952088</v>
+        <v>-60.65117239952087</v>
       </c>
     </row>
     <row r="36">
@@ -2014,19 +2014,19 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>1628786981</v>
+        <v>1629830951</v>
       </c>
       <c r="G36" t="b">
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I36" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J36" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K36" t="n">
         <v>-32.97151124878278</v>
@@ -2058,19 +2058,19 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>1628786995</v>
+        <v>1629830926</v>
       </c>
       <c r="G37" t="b">
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I37" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J37" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="K37" t="n">
         <v>-32.97084968284816</v>
@@ -2102,7 +2102,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>1628787001</v>
+        <v>1629830928</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
@@ -2111,10 +2111,10 @@
         <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J38" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K38" t="n">
         <v>-32.96977681526667</v>
@@ -2146,19 +2146,19 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>1628786987</v>
+        <v>1629830944</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J39" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K39" t="n">
         <v>-32.97733374029842</v>
@@ -2190,19 +2190,19 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>1628786981</v>
+        <v>1629830954</v>
       </c>
       <c r="G40" t="b">
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K40" t="n">
         <v>-32.95019913442736</v>
@@ -2234,19 +2234,19 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>1628786984</v>
+        <v>1629830922</v>
       </c>
       <c r="G41" t="b">
         <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J41" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="K41" t="n">
         <v>-32.92301479484789</v>
@@ -2278,19 +2278,19 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>1628786974</v>
+        <v>1629830953</v>
       </c>
       <c r="G42" t="b">
         <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J42" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K42" t="n">
         <v>-32.97468399612914</v>
@@ -2322,7 +2322,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>1628786979</v>
+        <v>1629830933</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
@@ -2331,10 +2331,10 @@
         <v>1</v>
       </c>
       <c r="I43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J43" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K43" t="n">
         <v>-32.9785541435317</v>
@@ -2366,19 +2366,19 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>1628786975</v>
+        <v>1629830948</v>
       </c>
       <c r="G44" t="b">
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K44" t="n">
         <v>-32.94441899725177</v>
@@ -2410,19 +2410,19 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>1628786975</v>
+        <v>1629830936</v>
       </c>
       <c r="G45" t="b">
         <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J45" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K45" t="n">
         <v>-32.95778386563791</v>
@@ -2454,19 +2454,19 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>1628786995</v>
+        <v>1629830950</v>
       </c>
       <c r="G46" t="b">
         <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J46" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K46" t="n">
         <v>-32.92653599347845</v>
@@ -2498,13 +2498,13 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>1628786974</v>
+        <v>1629830952</v>
       </c>
       <c r="G47" t="b">
         <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="n">
         <v>10</v>
@@ -2542,7 +2542,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>1628786988</v>
+        <v>1629830948</v>
       </c>
       <c r="G48" t="b">
         <v>0</v>
@@ -2551,10 +2551,10 @@
         <v>1</v>
       </c>
       <c r="I48" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J48" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K48" t="n">
         <v>-32.97858114396427</v>
@@ -2586,7 +2586,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>1628786982</v>
+        <v>1629830948</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
@@ -2595,10 +2595,10 @@
         <v>1</v>
       </c>
       <c r="I49" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J49" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K49" t="n">
         <v>-32.92171051403622</v>
@@ -2630,7 +2630,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>1628786997</v>
+        <v>1629830934</v>
       </c>
       <c r="G50" t="b">
         <v>0</v>
@@ -2674,7 +2674,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>1628786979</v>
+        <v>1629830925</v>
       </c>
       <c r="G51" t="b">
         <v>0</v>
@@ -2718,19 +2718,19 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>1628786973</v>
+        <v>1629830952</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J52" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K52" t="n">
         <v>-32.95708325593757</v>
@@ -2762,7 +2762,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>1628786976</v>
+        <v>1629830945</v>
       </c>
       <c r="G53" t="b">
         <v>0</v>
@@ -2771,10 +2771,10 @@
         <v>1</v>
       </c>
       <c r="I53" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J53" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K53" t="n">
         <v>-32.94759428718157</v>
@@ -2806,19 +2806,19 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>1628786973</v>
+        <v>1629830940</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
       </c>
       <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>17</v>
+      </c>
+      <c r="J54" t="n">
         <v>3</v>
-      </c>
-      <c r="I54" t="n">
-        <v>7</v>
-      </c>
-      <c r="J54" t="n">
-        <v>13</v>
       </c>
       <c r="K54" t="n">
         <v>-32.939457</v>
@@ -2850,19 +2850,19 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>1628786983</v>
+        <v>1629830932</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
       </c>
       <c r="H55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J55" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="K55" t="n">
         <v>-32.9581866</v>
@@ -2894,19 +2894,19 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>1628786981</v>
+        <v>1629830932</v>
       </c>
       <c r="G56" t="b">
         <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J56" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K56" t="n">
         <v>-32.9093257</v>
@@ -2938,7 +2938,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>1628786998</v>
+        <v>1629830949</v>
       </c>
       <c r="G57" t="b">
         <v>0</v>
@@ -2947,10 +2947,10 @@
         <v>0</v>
       </c>
       <c r="I57" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J57" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K57" t="n">
         <v>-32.91422795893311</v>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>1628786974</v>
+        <v>1629830951</v>
       </c>
       <c r="G58" t="b">
         <v>0</v>
@@ -2991,10 +2991,10 @@
         <v>0</v>
       </c>
       <c r="I58" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J58" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K58" t="n">
         <v>-32.89464556057717</v>
@@ -3026,16 +3026,16 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>1628786974</v>
+        <v>1629830938</v>
       </c>
       <c r="G59" t="b">
         <v>0</v>
       </c>
       <c r="H59" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I59" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J59" t="n">
         <v>3</v>
@@ -3070,19 +3070,19 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>1628786975</v>
+        <v>1629830930</v>
       </c>
       <c r="G60" t="b">
         <v>0</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I60" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J60" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="K60" t="n">
         <v>-32.91293717782394</v>
@@ -3114,19 +3114,19 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>1628786982</v>
+        <v>1629830941</v>
       </c>
       <c r="G61" t="b">
         <v>0</v>
       </c>
       <c r="H61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I61" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J61" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K61" t="n">
         <v>-32.89180515414552</v>
@@ -3158,7 +3158,7 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>1628786985</v>
+        <v>1629830942</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
@@ -3167,16 +3167,16 @@
         <v>1</v>
       </c>
       <c r="I62" t="n">
+        <v>11</v>
+      </c>
+      <c r="J62" t="n">
         <v>9</v>
-      </c>
-      <c r="J62" t="n">
-        <v>11</v>
       </c>
       <c r="K62" t="n">
         <v>-32.88490773761225</v>
       </c>
       <c r="L62" t="n">
-        <v>-60.68735302130976</v>
+        <v>-60.68735302130975</v>
       </c>
     </row>
     <row r="63">
@@ -3202,7 +3202,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>1628786986</v>
+        <v>1629830940</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
@@ -3211,10 +3211,10 @@
         <v>0</v>
       </c>
       <c r="I63" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J63" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K63" t="n">
         <v>-32.910503</v>
@@ -3246,7 +3246,7 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>1628787001</v>
+        <v>1629830949</v>
       </c>
       <c r="G64" t="b">
         <v>0</v>
@@ -3255,10 +3255,10 @@
         <v>0</v>
       </c>
       <c r="I64" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J64" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K64" t="n">
         <v>-32.90654927658849</v>
@@ -3290,19 +3290,19 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>1628786981</v>
+        <v>1629830934</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
       </c>
       <c r="H65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J65" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K65" t="n">
         <v>-32.942375</v>
@@ -3334,19 +3334,19 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>1628787000</v>
+        <v>1629830931</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>
       </c>
       <c r="H66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J66" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K66" t="n">
         <v>-32.941427</v>
@@ -3378,19 +3378,19 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>1628786984</v>
+        <v>1629830938</v>
       </c>
       <c r="G67" t="b">
         <v>0</v>
       </c>
       <c r="H67" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I67" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J67" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K67" t="n">
         <v>-32.940079</v>
@@ -3422,19 +3422,19 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>1628786996</v>
+        <v>1629830946</v>
       </c>
       <c r="G68" t="b">
         <v>0</v>
       </c>
       <c r="H68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="J68" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="K68" t="n">
         <v>-32.940247</v>
@@ -3466,7 +3466,7 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>1628786992</v>
+        <v>1629830945</v>
       </c>
       <c r="G69" t="b">
         <v>0</v>
@@ -3475,10 +3475,10 @@
         <v>0</v>
       </c>
       <c r="I69" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J69" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K69" t="n">
         <v>-32.933226</v>
@@ -3510,19 +3510,19 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>1628786977</v>
+        <v>1629830942</v>
       </c>
       <c r="G70" t="b">
         <v>0</v>
       </c>
       <c r="H70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" t="n">
+        <v>8</v>
+      </c>
+      <c r="J70" t="n">
         <v>11</v>
-      </c>
-      <c r="J70" t="n">
-        <v>9</v>
       </c>
       <c r="K70" t="n">
         <v>-32.928205</v>
@@ -3554,19 +3554,19 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>1628786998</v>
+        <v>1629830940</v>
       </c>
       <c r="G71" t="b">
         <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I71" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="J71" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="K71" t="n">
         <v>-32.8736414</v>

</xml_diff>

<commit_message>
fix logic + base de datos de prueba
</commit_message>
<xml_diff>
--- a/datos/geo/estaciones.xlsx
+++ b/datos/geo/estaciones.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,40 +456,25 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>anchor</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>last_connection_date</t>
+          <t>bikes</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>favorite</t>
+          <t>capacity</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>tandem</t>
+          <t>latitude</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>anchor</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>bikes</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>latitude</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>longitude</t>
         </is>
@@ -512,30 +497,19 @@
       <c r="D2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E2" t="n">
+        <v>19</v>
       </c>
       <c r="F2" t="n">
-        <v>1631236298</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>20</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>-32.95421439665977</v>
       </c>
       <c r="I2" t="n">
-        <v>13</v>
-      </c>
-      <c r="J2" t="n">
-        <v>7</v>
-      </c>
-      <c r="K2" t="n">
-        <v>-32.95421439665977</v>
-      </c>
-      <c r="L2" t="n">
         <v>-60.65598696470261</v>
       </c>
     </row>
@@ -556,30 +530,19 @@
       <c r="D3" t="n">
         <v>2</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E3" t="n">
+        <v>8</v>
       </c>
       <c r="F3" t="n">
-        <v>1631236302</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="G3" t="n">
+        <v>20</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>-32.95666307690848</v>
       </c>
       <c r="I3" t="n">
-        <v>12</v>
-      </c>
-      <c r="J3" t="n">
-        <v>7</v>
-      </c>
-      <c r="K3" t="n">
-        <v>-32.95666307690848</v>
-      </c>
-      <c r="L3" t="n">
         <v>-60.64486920833588</v>
       </c>
     </row>
@@ -600,30 +563,19 @@
       <c r="D4" t="n">
         <v>3</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E4" t="n">
+        <v>12</v>
       </c>
       <c r="F4" t="n">
-        <v>1631236276</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="G4" t="n">
+        <v>20</v>
       </c>
       <c r="H4" t="n">
-        <v>2</v>
+        <v>-32.95812144981906</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>19</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-32.95812144981906</v>
-      </c>
-      <c r="L4" t="n">
         <v>-60.63670188188553</v>
       </c>
     </row>
@@ -644,30 +596,19 @@
       <c r="D5" t="n">
         <v>4</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E5" t="n">
+        <v>13</v>
       </c>
       <c r="F5" t="n">
-        <v>1631236294</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G5" t="n">
+        <v>22</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>-32.95921521370776</v>
       </c>
       <c r="I5" t="n">
-        <v>10</v>
-      </c>
-      <c r="J5" t="n">
-        <v>10</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-32.95921521370776</v>
-      </c>
-      <c r="L5" t="n">
         <v>-60.62944918870926</v>
       </c>
     </row>
@@ -688,30 +629,19 @@
       <c r="D6" t="n">
         <v>5</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E6" t="n">
+        <v>15</v>
       </c>
       <c r="F6" t="n">
-        <v>1631236300</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G6" t="n">
+        <v>21</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>-32.96736625395059</v>
       </c>
       <c r="I6" t="n">
-        <v>15</v>
-      </c>
-      <c r="J6" t="n">
-        <v>6</v>
-      </c>
-      <c r="K6" t="n">
-        <v>-32.96736625395059</v>
-      </c>
-      <c r="L6" t="n">
         <v>-60.62357246875763</v>
       </c>
     </row>
@@ -732,30 +662,19 @@
       <c r="D7" t="n">
         <v>6</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E7" t="n">
+        <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>1631236279</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="G7" t="n">
+        <v>16</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>-32.96850040867347</v>
       </c>
       <c r="I7" t="n">
-        <v>15</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>-32.96850040867347</v>
-      </c>
-      <c r="L7" t="n">
         <v>-60.62398016452789</v>
       </c>
     </row>
@@ -776,30 +695,19 @@
       <c r="D8" t="n">
         <v>7</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E8" t="n">
+        <v>17</v>
       </c>
       <c r="F8" t="n">
-        <v>1631236295</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G8" t="n">
+        <v>23</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>-32.93944885753075</v>
       </c>
       <c r="I8" t="n">
-        <v>10</v>
-      </c>
-      <c r="J8" t="n">
-        <v>11</v>
-      </c>
-      <c r="K8" t="n">
-        <v>-32.93944885753075</v>
-      </c>
-      <c r="L8" t="n">
         <v>-60.67054331302643</v>
       </c>
     </row>
@@ -820,30 +728,19 @@
       <c r="D9" t="n">
         <v>8</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E9" t="n">
+        <v>12</v>
       </c>
       <c r="F9" t="n">
-        <v>1631236280</v>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G9" t="n">
+        <v>16</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>-32.9403492658816</v>
       </c>
       <c r="I9" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" t="n">
-        <v>14</v>
-      </c>
-      <c r="K9" t="n">
-        <v>-32.9403492658816</v>
-      </c>
-      <c r="L9" t="n">
         <v>-60.665243268013</v>
       </c>
     </row>
@@ -864,30 +761,19 @@
       <c r="D10" t="n">
         <v>9</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E10" t="n">
+        <v>9</v>
       </c>
       <c r="F10" t="n">
-        <v>1631236290</v>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>10</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>-32.94573801821987</v>
       </c>
       <c r="I10" t="n">
-        <v>8</v>
-      </c>
-      <c r="J10" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" t="n">
-        <v>-32.94573801821987</v>
-      </c>
-      <c r="L10" t="n">
         <v>-60.65809518098831</v>
       </c>
     </row>
@@ -908,30 +794,19 @@
       <c r="D11" t="n">
         <v>10</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E11" t="n">
+        <v>19</v>
       </c>
       <c r="F11" t="n">
-        <v>1631236293</v>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>20</v>
       </c>
       <c r="H11" t="n">
-        <v>2</v>
+        <v>-32.94996730598237</v>
       </c>
       <c r="I11" t="n">
-        <v>7</v>
-      </c>
-      <c r="J11" t="n">
-        <v>13</v>
-      </c>
-      <c r="K11" t="n">
-        <v>-32.94996730598237</v>
-      </c>
-      <c r="L11" t="n">
         <v>-60.65478533506393</v>
       </c>
     </row>
@@ -952,30 +827,19 @@
       <c r="D12" t="n">
         <v>11</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E12" t="n">
+        <v>4</v>
       </c>
       <c r="F12" t="n">
-        <v>1631236303</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G12" t="n">
+        <v>18</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>-32.94402733877261</v>
       </c>
       <c r="I12" t="n">
-        <v>7</v>
-      </c>
-      <c r="J12" t="n">
-        <v>11</v>
-      </c>
-      <c r="K12" t="n">
-        <v>-32.94402733877261</v>
-      </c>
-      <c r="L12" t="n">
         <v>-60.65053671598434</v>
       </c>
     </row>
@@ -996,30 +860,19 @@
       <c r="D13" t="n">
         <v>12</v>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E13" t="n">
+        <v>4</v>
       </c>
       <c r="F13" t="n">
-        <v>1631236284</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="G13" t="n">
+        <v>21</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>-32.94531035146112</v>
       </c>
       <c r="I13" t="n">
-        <v>15</v>
-      </c>
-      <c r="J13" t="n">
-        <v>5</v>
-      </c>
-      <c r="K13" t="n">
-        <v>-32.94531035146112</v>
-      </c>
-      <c r="L13" t="n">
         <v>-60.64449772238731</v>
       </c>
     </row>
@@ -1040,30 +893,19 @@
       <c r="D14" t="n">
         <v>14</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E14" t="n">
+        <v>12</v>
       </c>
       <c r="F14" t="n">
-        <v>1631236280</v>
-      </c>
-      <c r="G14" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G14" t="n">
+        <v>21</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>-32.9493843560409</v>
       </c>
       <c r="I14" t="n">
-        <v>13</v>
-      </c>
-      <c r="J14" t="n">
-        <v>8</v>
-      </c>
-      <c r="K14" t="n">
-        <v>-32.9493843560409</v>
-      </c>
-      <c r="L14" t="n">
         <v>-60.63740864396095</v>
       </c>
     </row>
@@ -1084,30 +926,19 @@
       <c r="D15" t="n">
         <v>13</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E15" t="n">
+        <v>10</v>
       </c>
       <c r="F15" t="n">
-        <v>1631236281</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="G15" t="n">
+        <v>21</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>-32.94882616098827</v>
       </c>
       <c r="I15" t="n">
-        <v>19</v>
-      </c>
-      <c r="J15" t="n">
-        <v>1</v>
-      </c>
-      <c r="K15" t="n">
-        <v>-32.94882616098827</v>
-      </c>
-      <c r="L15" t="n">
         <v>-60.64177662134171</v>
       </c>
     </row>
@@ -1128,30 +959,19 @@
       <c r="D16" t="n">
         <v>15</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E16" t="n">
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>1631236298</v>
-      </c>
-      <c r="G16" t="b">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="G16" t="n">
+        <v>20</v>
       </c>
       <c r="H16" t="n">
-        <v>2</v>
+        <v>-32.94755220262625</v>
       </c>
       <c r="I16" t="n">
-        <v>3</v>
-      </c>
-      <c r="J16" t="n">
-        <v>17</v>
-      </c>
-      <c r="K16" t="n">
-        <v>-32.94755220262625</v>
-      </c>
-      <c r="L16" t="n">
         <v>-60.63288778066635</v>
       </c>
     </row>
@@ -1172,30 +992,19 @@
       <c r="D17" t="n">
         <v>16</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E17" t="n">
+        <v>8</v>
       </c>
       <c r="F17" t="n">
-        <v>1631236285</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="G17" t="n">
+        <v>20</v>
       </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>-32.93659000025387</v>
       </c>
       <c r="I17" t="n">
-        <v>10</v>
-      </c>
-      <c r="J17" t="n">
-        <v>10</v>
-      </c>
-      <c r="K17" t="n">
-        <v>-32.93659000025387</v>
-      </c>
-      <c r="L17" t="n">
         <v>-60.65140575170517</v>
       </c>
     </row>
@@ -1216,30 +1025,19 @@
       <c r="D18" t="n">
         <v>17</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E18" t="n">
+        <v>9</v>
       </c>
       <c r="F18" t="n">
-        <v>1631236288</v>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="G18" t="n">
+        <v>19</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>-32.93587864817957</v>
       </c>
       <c r="I18" t="n">
-        <v>9</v>
-      </c>
-      <c r="J18" t="n">
-        <v>11</v>
-      </c>
-      <c r="K18" t="n">
-        <v>-32.93587864817957</v>
-      </c>
-      <c r="L18" t="n">
         <v>-60.64261347055435</v>
       </c>
     </row>
@@ -1260,30 +1058,19 @@
       <c r="D19" t="n">
         <v>18</v>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E19" t="n">
+        <v>12</v>
       </c>
       <c r="F19" t="n">
-        <v>1631236299</v>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="G19" t="n">
+        <v>19</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>-32.94099755421734</v>
       </c>
       <c r="I19" t="n">
-        <v>12</v>
-      </c>
-      <c r="J19" t="n">
-        <v>7</v>
-      </c>
-      <c r="K19" t="n">
-        <v>-32.94099755421734</v>
-      </c>
-      <c r="L19" t="n">
         <v>-60.63473045825958</v>
       </c>
     </row>
@@ -1304,30 +1091,19 @@
       <c r="D20" t="n">
         <v>19</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E20" t="n">
+        <v>5</v>
       </c>
       <c r="F20" t="n">
-        <v>1631236281</v>
-      </c>
-      <c r="G20" t="b">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="G20" t="n">
+        <v>12</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>-32.95358421061909</v>
       </c>
       <c r="I20" t="n">
-        <v>8</v>
-      </c>
-      <c r="J20" t="n">
-        <v>4</v>
-      </c>
-      <c r="K20" t="n">
-        <v>-32.95358421061909</v>
-      </c>
-      <c r="L20" t="n">
         <v>-60.66343545913696</v>
       </c>
     </row>
@@ -1348,30 +1124,19 @@
       <c r="D21" t="n">
         <v>33</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E21" t="n">
+        <v>19</v>
       </c>
       <c r="F21" t="n">
-        <v>1631236295</v>
-      </c>
-      <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>20</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>-32.95206724436681</v>
       </c>
       <c r="I21" t="n">
-        <v>10</v>
-      </c>
-      <c r="J21" t="n">
-        <v>10</v>
-      </c>
-      <c r="K21" t="n">
-        <v>-32.95206724436681</v>
-      </c>
-      <c r="L21" t="n">
         <v>-60.67079275846481</v>
       </c>
     </row>
@@ -1392,30 +1157,19 @@
       <c r="D22" t="n">
         <v>31</v>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E22" t="n">
+        <v>9</v>
       </c>
       <c r="F22" t="n">
-        <v>1631236276</v>
-      </c>
-      <c r="G22" t="b">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>-32.96512040461018</v>
       </c>
       <c r="I22" t="n">
-        <v>10</v>
-      </c>
-      <c r="J22" t="n">
-        <v>10</v>
-      </c>
-      <c r="K22" t="n">
-        <v>-32.96512040461018</v>
-      </c>
-      <c r="L22" t="n">
         <v>-60.65592795610428</v>
       </c>
     </row>
@@ -1436,30 +1190,19 @@
       <c r="D23" t="n">
         <v>36</v>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E23" t="n">
+        <v>7</v>
       </c>
       <c r="F23" t="n">
-        <v>1631236293</v>
-      </c>
-      <c r="G23" t="b">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="G23" t="n">
+        <v>20</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>-32.92663505330592</v>
       </c>
       <c r="I23" t="n">
-        <v>11</v>
-      </c>
-      <c r="J23" t="n">
-        <v>9</v>
-      </c>
-      <c r="K23" t="n">
-        <v>-32.92663505330592</v>
-      </c>
-      <c r="L23" t="n">
         <v>-60.65880596637726</v>
       </c>
     </row>
@@ -1480,30 +1223,19 @@
       <c r="D24" t="n">
         <v>28</v>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E24" t="n">
+        <v>13</v>
       </c>
       <c r="F24" t="n">
-        <v>1631236294</v>
-      </c>
-      <c r="G24" t="b">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="G24" t="n">
+        <v>20</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>-32.93184904583995</v>
       </c>
       <c r="I24" t="n">
-        <v>15</v>
-      </c>
-      <c r="J24" t="n">
-        <v>5</v>
-      </c>
-      <c r="K24" t="n">
-        <v>-32.93184904583995</v>
-      </c>
-      <c r="L24" t="n">
         <v>-60.65018132328987</v>
       </c>
     </row>
@@ -1524,30 +1256,19 @@
       <c r="D25" t="n">
         <v>26</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E25" t="n">
+        <v>16</v>
       </c>
       <c r="F25" t="n">
-        <v>1631236274</v>
-      </c>
-      <c r="G25" t="b">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G25" t="n">
+        <v>20</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>-32.94041229412281</v>
       </c>
       <c r="I25" t="n">
-        <v>17</v>
-      </c>
-      <c r="J25" t="n">
-        <v>3</v>
-      </c>
-      <c r="K25" t="n">
-        <v>-32.94041229412281</v>
-      </c>
-      <c r="L25" t="n">
         <v>-60.64960062503815</v>
       </c>
     </row>
@@ -1568,30 +1289,19 @@
       <c r="D26" t="n">
         <v>21</v>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E26" t="n">
+        <v>11</v>
       </c>
       <c r="F26" t="n">
-        <v>1631236288</v>
-      </c>
-      <c r="G26" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G26" t="n">
+        <v>20</v>
       </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>-32.96268096048085</v>
       </c>
       <c r="I26" t="n">
-        <v>14</v>
-      </c>
-      <c r="J26" t="n">
-        <v>6</v>
-      </c>
-      <c r="K26" t="n">
-        <v>-32.96268096048085</v>
-      </c>
-      <c r="L26" t="n">
         <v>-60.64523935317993</v>
       </c>
     </row>
@@ -1612,30 +1322,19 @@
       <c r="D27" t="n">
         <v>32</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E27" t="n">
+        <v>11</v>
       </c>
       <c r="F27" t="n">
-        <v>1631236173</v>
-      </c>
-      <c r="G27" t="b">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G27" t="n">
+        <v>15</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>-32.96806835144843</v>
       </c>
       <c r="I27" t="n">
-        <v>13</v>
-      </c>
-      <c r="J27" t="n">
-        <v>2</v>
-      </c>
-      <c r="K27" t="n">
-        <v>-32.96806835144843</v>
-      </c>
-      <c r="L27" t="n">
         <v>-60.64059376716614</v>
       </c>
     </row>
@@ -1656,30 +1355,19 @@
       <c r="D28" t="n">
         <v>22</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E28" t="n">
+        <v>12</v>
       </c>
       <c r="F28" t="n">
-        <v>1631236297</v>
-      </c>
-      <c r="G28" t="b">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="G28" t="n">
+        <v>20</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>-32.96399070730771</v>
       </c>
       <c r="I28" t="n">
-        <v>4</v>
-      </c>
-      <c r="J28" t="n">
-        <v>16</v>
-      </c>
-      <c r="K28" t="n">
-        <v>-32.96399070730771</v>
-      </c>
-      <c r="L28" t="n">
         <v>-60.63680648803711</v>
       </c>
     </row>
@@ -1700,30 +1388,19 @@
       <c r="D29" t="n">
         <v>24</v>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E29" t="n">
+        <v>8</v>
       </c>
       <c r="F29" t="n">
-        <v>1631236295</v>
-      </c>
-      <c r="G29" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G29" t="n">
+        <v>17</v>
       </c>
       <c r="H29" t="n">
-        <v>1</v>
+        <v>-32.95339515393067</v>
       </c>
       <c r="I29" t="n">
-        <v>8</v>
-      </c>
-      <c r="J29" t="n">
-        <v>7</v>
-      </c>
-      <c r="K29" t="n">
-        <v>-32.95339515393067</v>
-      </c>
-      <c r="L29" t="n">
         <v>-60.62930703163147</v>
       </c>
     </row>
@@ -1744,30 +1421,19 @@
       <c r="D30" t="n">
         <v>25</v>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E30" t="n">
+        <v>12</v>
       </c>
       <c r="F30" t="n">
-        <v>1631236276</v>
-      </c>
-      <c r="G30" t="b">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="G30" t="n">
+        <v>20</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>-32.93516278810112</v>
       </c>
       <c r="I30" t="n">
-        <v>17</v>
-      </c>
-      <c r="J30" t="n">
-        <v>3</v>
-      </c>
-      <c r="K30" t="n">
-        <v>-32.93516278810112</v>
-      </c>
-      <c r="L30" t="n">
         <v>-60.65977692604065</v>
       </c>
     </row>
@@ -1788,30 +1454,19 @@
       <c r="D31" t="n">
         <v>27</v>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E31" t="n">
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>1631236287</v>
-      </c>
-      <c r="G31" t="b">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="G31" t="n">
+        <v>22</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>-32.94162782998716</v>
       </c>
       <c r="I31" t="n">
-        <v>19</v>
-      </c>
-      <c r="J31" t="n">
-        <v>1</v>
-      </c>
-      <c r="K31" t="n">
-        <v>-32.94162782998716</v>
-      </c>
-      <c r="L31" t="n">
         <v>-60.63880205154419</v>
       </c>
     </row>
@@ -1832,30 +1487,19 @@
       <c r="D32" t="n">
         <v>29</v>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E32" t="n">
+        <v>6</v>
       </c>
       <c r="F32" t="n">
-        <v>1631236300</v>
-      </c>
-      <c r="G32" t="b">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="G32" t="n">
+        <v>14</v>
       </c>
       <c r="H32" t="n">
-        <v>1</v>
+        <v>-32.95894064873677</v>
       </c>
       <c r="I32" t="n">
-        <v>6</v>
-      </c>
-      <c r="J32" t="n">
-        <v>6</v>
-      </c>
-      <c r="K32" t="n">
-        <v>-32.95894064873677</v>
-      </c>
-      <c r="L32" t="n">
         <v>-60.67002296447754</v>
       </c>
     </row>
@@ -1876,30 +1520,19 @@
       <c r="D33" t="n">
         <v>30</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E33" t="n">
+        <v>12</v>
       </c>
       <c r="F33" t="n">
-        <v>1631236275</v>
-      </c>
-      <c r="G33" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G33" t="n">
+        <v>21</v>
       </c>
       <c r="H33" t="n">
-        <v>3</v>
+        <v>-32.96361263805213</v>
       </c>
       <c r="I33" t="n">
-        <v>6</v>
-      </c>
-      <c r="J33" t="n">
-        <v>14</v>
-      </c>
-      <c r="K33" t="n">
-        <v>-32.96361263805213</v>
-      </c>
-      <c r="L33" t="n">
         <v>-60.66525936126709</v>
       </c>
     </row>
@@ -1920,30 +1553,19 @@
       <c r="D34" t="n">
         <v>34</v>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E34" t="n">
+        <v>17</v>
       </c>
       <c r="F34" t="n">
-        <v>1631236300</v>
-      </c>
-      <c r="G34" t="b">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G34" t="n">
+        <v>20</v>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>-32.94575602519591</v>
       </c>
       <c r="I34" t="n">
-        <v>7</v>
-      </c>
-      <c r="J34" t="n">
-        <v>13</v>
-      </c>
-      <c r="K34" t="n">
-        <v>-32.94575602519591</v>
-      </c>
-      <c r="L34" t="n">
         <v>-60.6721043586731</v>
       </c>
     </row>
@@ -1964,30 +1586,19 @@
       <c r="D35" t="n">
         <v>20</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E35" t="n">
+        <v>17</v>
       </c>
       <c r="F35" t="n">
-        <v>1631236276</v>
-      </c>
-      <c r="G35" t="b">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G35" t="n">
+        <v>20</v>
       </c>
       <c r="H35" t="n">
-        <v>2</v>
+        <v>-32.9556277975818</v>
       </c>
       <c r="I35" t="n">
-        <v>9</v>
-      </c>
-      <c r="J35" t="n">
-        <v>11</v>
-      </c>
-      <c r="K35" t="n">
-        <v>-32.9556277975818</v>
-      </c>
-      <c r="L35" t="n">
         <v>-60.65117239952087</v>
       </c>
     </row>
@@ -2008,30 +1619,19 @@
       <c r="D36" t="n">
         <v>49</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E36" t="n">
+        <v>10</v>
       </c>
       <c r="F36" t="n">
-        <v>1631236275</v>
-      </c>
-      <c r="G36" t="b">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G36" t="n">
+        <v>16</v>
       </c>
       <c r="H36" t="n">
-        <v>2</v>
+        <v>-32.97151124878278</v>
       </c>
       <c r="I36" t="n">
-        <v>12</v>
-      </c>
-      <c r="J36" t="n">
-        <v>4</v>
-      </c>
-      <c r="K36" t="n">
-        <v>-32.97151124878278</v>
-      </c>
-      <c r="L36" t="n">
         <v>-60.6603080034256</v>
       </c>
     </row>
@@ -2052,30 +1652,19 @@
       <c r="D37" t="n">
         <v>37</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E37" t="n">
+        <v>16</v>
       </c>
       <c r="F37" t="n">
-        <v>1631236300</v>
-      </c>
-      <c r="G37" t="b">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G37" t="n">
+        <v>20</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>-32.97084968284816</v>
       </c>
       <c r="I37" t="n">
-        <v>16</v>
-      </c>
-      <c r="J37" t="n">
-        <v>4</v>
-      </c>
-      <c r="K37" t="n">
-        <v>-32.97084968284816</v>
-      </c>
-      <c r="L37" t="n">
         <v>-60.64461708068848</v>
       </c>
     </row>
@@ -2096,30 +1685,19 @@
       <c r="D38" t="n">
         <v>38</v>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E38" t="n">
+        <v>16</v>
       </c>
       <c r="F38" t="n">
-        <v>1631236300</v>
-      </c>
-      <c r="G38" t="b">
         <v>0</v>
       </c>
+      <c r="G38" t="n">
+        <v>16</v>
+      </c>
       <c r="H38" t="n">
-        <v>2</v>
+        <v>-32.96977681526667</v>
       </c>
       <c r="I38" t="n">
-        <v>11</v>
-      </c>
-      <c r="J38" t="n">
-        <v>5</v>
-      </c>
-      <c r="K38" t="n">
-        <v>-32.96977681526667</v>
-      </c>
-      <c r="L38" t="n">
         <v>-60.63395261764526</v>
       </c>
     </row>
@@ -2140,30 +1718,19 @@
       <c r="D39" t="n">
         <v>51</v>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E39" t="n">
+        <v>11</v>
       </c>
       <c r="F39" t="n">
-        <v>1631236293</v>
-      </c>
-      <c r="G39" t="b">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="G39" t="n">
+        <v>16</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>-32.97733374029842</v>
       </c>
       <c r="I39" t="n">
-        <v>10</v>
-      </c>
-      <c r="J39" t="n">
-        <v>6</v>
-      </c>
-      <c r="K39" t="n">
-        <v>-32.97733374029842</v>
-      </c>
-      <c r="L39" t="n">
         <v>-60.64409136772156</v>
       </c>
     </row>
@@ -2184,30 +1751,19 @@
       <c r="D40" t="n">
         <v>41</v>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E40" t="n">
+        <v>11</v>
       </c>
       <c r="F40" t="n">
-        <v>1631236293</v>
-      </c>
-      <c r="G40" t="b">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G40" t="n">
+        <v>13</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>-32.95019913442736</v>
       </c>
       <c r="I40" t="n">
-        <v>7</v>
-      </c>
-      <c r="J40" t="n">
-        <v>5</v>
-      </c>
-      <c r="K40" t="n">
-        <v>-32.95019913442736</v>
-      </c>
-      <c r="L40" t="n">
         <v>-60.68156719207764</v>
       </c>
     </row>
@@ -2228,30 +1784,19 @@
       <c r="D41" t="n">
         <v>44</v>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E41" t="n">
+        <v>6</v>
       </c>
       <c r="F41" t="n">
-        <v>1631236298</v>
-      </c>
-      <c r="G41" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G41" t="n">
+        <v>21</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>-32.92301479484789</v>
       </c>
       <c r="I41" t="n">
-        <v>16</v>
-      </c>
-      <c r="J41" t="n">
-        <v>4</v>
-      </c>
-      <c r="K41" t="n">
-        <v>-32.92301479484789</v>
-      </c>
-      <c r="L41" t="n">
         <v>-60.66567778587341</v>
       </c>
     </row>
@@ -2272,30 +1817,19 @@
       <c r="D42" t="n">
         <v>47</v>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E42" t="n">
+        <v>9</v>
       </c>
       <c r="F42" t="n">
-        <v>1631236293</v>
-      </c>
-      <c r="G42" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="G42" t="n">
+        <v>19</v>
       </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>-32.97468399612914</v>
       </c>
       <c r="I42" t="n">
-        <v>6</v>
-      </c>
-      <c r="J42" t="n">
-        <v>10</v>
-      </c>
-      <c r="K42" t="n">
-        <v>-32.97468399612914</v>
-      </c>
-      <c r="L42" t="n">
         <v>-60.66910028457642</v>
       </c>
     </row>
@@ -2316,30 +1850,19 @@
       <c r="D43" t="n">
         <v>50</v>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E43" t="n">
+        <v>8</v>
       </c>
       <c r="F43" t="n">
-        <v>1631236296</v>
-      </c>
-      <c r="G43" t="b">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="G43" t="n">
+        <v>16</v>
       </c>
       <c r="H43" t="n">
-        <v>1</v>
+        <v>-32.9785541435317</v>
       </c>
       <c r="I43" t="n">
-        <v>8</v>
-      </c>
-      <c r="J43" t="n">
-        <v>8</v>
-      </c>
-      <c r="K43" t="n">
-        <v>-32.9785541435317</v>
-      </c>
-      <c r="L43" t="n">
         <v>-60.64939141273499</v>
       </c>
     </row>
@@ -2360,30 +1883,19 @@
       <c r="D44" t="n">
         <v>45</v>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E44" t="n">
+        <v>13</v>
       </c>
       <c r="F44" t="n">
-        <v>1631236292</v>
-      </c>
-      <c r="G44" t="b">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="G44" t="n">
+        <v>20</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>-32.94441899725177</v>
       </c>
       <c r="I44" t="n">
-        <v>14</v>
-      </c>
-      <c r="J44" t="n">
-        <v>6</v>
-      </c>
-      <c r="K44" t="n">
-        <v>-32.94441899725177</v>
-      </c>
-      <c r="L44" t="n">
         <v>-60.68002223968506</v>
       </c>
     </row>
@@ -2404,30 +1916,19 @@
       <c r="D45" t="n">
         <v>39</v>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E45" t="n">
+        <v>9</v>
       </c>
       <c r="F45" t="n">
-        <v>1631236279</v>
-      </c>
-      <c r="G45" t="b">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G45" t="n">
+        <v>12</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>-32.95778386563791</v>
       </c>
       <c r="I45" t="n">
-        <v>8</v>
-      </c>
-      <c r="J45" t="n">
-        <v>4</v>
-      </c>
-      <c r="K45" t="n">
-        <v>-32.95778386563791</v>
-      </c>
-      <c r="L45" t="n">
         <v>-60.68373441696167</v>
       </c>
     </row>
@@ -2448,30 +1949,19 @@
       <c r="D46" t="n">
         <v>43</v>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E46" t="n">
+        <v>11</v>
       </c>
       <c r="F46" t="n">
-        <v>1631236284</v>
-      </c>
-      <c r="G46" t="b">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="G46" t="n">
+        <v>22</v>
       </c>
       <c r="H46" t="n">
-        <v>2</v>
+        <v>-32.92653599347845</v>
       </c>
       <c r="I46" t="n">
-        <v>12</v>
-      </c>
-      <c r="J46" t="n">
-        <v>8</v>
-      </c>
-      <c r="K46" t="n">
-        <v>-32.92653599347845</v>
-      </c>
-      <c r="L46" t="n">
         <v>-60.6690788269043</v>
       </c>
     </row>
@@ -2492,30 +1982,19 @@
       <c r="D47" t="n">
         <v>48</v>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E47" t="n">
+        <v>7</v>
       </c>
       <c r="F47" t="n">
-        <v>1631236276</v>
-      </c>
-      <c r="G47" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G47" t="n">
+        <v>16</v>
       </c>
       <c r="H47" t="n">
-        <v>2</v>
+        <v>-32.97646608507204</v>
       </c>
       <c r="I47" t="n">
-        <v>4</v>
-      </c>
-      <c r="J47" t="n">
-        <v>12</v>
-      </c>
-      <c r="K47" t="n">
-        <v>-32.97646608507204</v>
-      </c>
-      <c r="L47" t="n">
         <v>-60.66103219985962</v>
       </c>
     </row>
@@ -2536,30 +2015,19 @@
       <c r="D48" t="n">
         <v>52</v>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E48" t="n">
+        <v>12</v>
       </c>
       <c r="F48" t="n">
-        <v>1631236276</v>
-      </c>
-      <c r="G48" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G48" t="n">
+        <v>21</v>
       </c>
       <c r="H48" t="n">
-        <v>1</v>
+        <v>-32.97858114396427</v>
       </c>
       <c r="I48" t="n">
-        <v>7</v>
-      </c>
-      <c r="J48" t="n">
-        <v>13</v>
-      </c>
-      <c r="K48" t="n">
-        <v>-32.97858114396427</v>
-      </c>
-      <c r="L48" t="n">
         <v>-60.63432276248932</v>
       </c>
     </row>
@@ -2580,30 +2048,19 @@
       <c r="D49" t="n">
         <v>42</v>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E49" t="n">
+        <v>14</v>
       </c>
       <c r="F49" t="n">
-        <v>1631236297</v>
-      </c>
-      <c r="G49" t="b">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G49" t="n">
+        <v>16</v>
       </c>
       <c r="H49" t="n">
-        <v>1</v>
+        <v>-32.92171051403622</v>
       </c>
       <c r="I49" t="n">
-        <v>11</v>
-      </c>
-      <c r="J49" t="n">
-        <v>5</v>
-      </c>
-      <c r="K49" t="n">
-        <v>-32.92171051403622</v>
-      </c>
-      <c r="L49" t="n">
         <v>-60.67459104854584</v>
       </c>
     </row>
@@ -2624,30 +2081,19 @@
       <c r="D50" t="n">
         <v>46</v>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E50" t="n">
+        <v>11</v>
       </c>
       <c r="F50" t="n">
-        <v>1631236298</v>
-      </c>
-      <c r="G50" t="b">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G50" t="n">
+        <v>17</v>
       </c>
       <c r="H50" t="n">
-        <v>2</v>
+        <v>-32.91607261912905</v>
       </c>
       <c r="I50" t="n">
-        <v>7</v>
-      </c>
-      <c r="J50" t="n">
-        <v>9</v>
-      </c>
-      <c r="K50" t="n">
-        <v>-32.91607261912905</v>
-      </c>
-      <c r="L50" t="n">
         <v>-60.67317350108146</v>
       </c>
     </row>
@@ -2668,30 +2114,19 @@
       <c r="D51" t="n">
         <v>35</v>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E51" t="n">
+        <v>16</v>
       </c>
       <c r="F51" t="n">
-        <v>1631236297</v>
-      </c>
-      <c r="G51" t="b">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G51" t="n">
+        <v>22</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>-32.93410631523491</v>
       </c>
       <c r="I51" t="n">
-        <v>13</v>
-      </c>
-      <c r="J51" t="n">
-        <v>7</v>
-      </c>
-      <c r="K51" t="n">
-        <v>-32.93410631523491</v>
-      </c>
-      <c r="L51" t="n">
         <v>-60.66570220787048</v>
       </c>
     </row>
@@ -2712,30 +2147,19 @@
       <c r="D52" t="n">
         <v>40</v>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E52" t="n">
+        <v>4</v>
       </c>
       <c r="F52" t="n">
-        <v>1631236282</v>
-      </c>
-      <c r="G52" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="G52" t="n">
+        <v>14</v>
       </c>
       <c r="H52" t="n">
-        <v>0</v>
+        <v>-32.95708325593757</v>
       </c>
       <c r="I52" t="n">
-        <v>5</v>
-      </c>
-      <c r="J52" t="n">
-        <v>7</v>
-      </c>
-      <c r="K52" t="n">
-        <v>-32.95708325593757</v>
-      </c>
-      <c r="L52" t="n">
         <v>-60.67632375556946</v>
       </c>
     </row>
@@ -2756,30 +2180,19 @@
       <c r="D53" t="n">
         <v>23</v>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E53" t="n">
+        <v>15</v>
       </c>
       <c r="F53" t="n">
-        <v>1631236298</v>
-      </c>
-      <c r="G53" t="b">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G53" t="n">
+        <v>21</v>
       </c>
       <c r="H53" t="n">
-        <v>2</v>
+        <v>-32.94759428718157</v>
       </c>
       <c r="I53" t="n">
-        <v>7</v>
-      </c>
-      <c r="J53" t="n">
-        <v>13</v>
-      </c>
-      <c r="K53" t="n">
-        <v>-32.94759428718157</v>
-      </c>
-      <c r="L53" t="n">
         <v>-60.6621026833725</v>
       </c>
     </row>
@@ -2800,30 +2213,19 @@
       <c r="D54" t="n">
         <v>53</v>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E54" t="n">
+        <v>18</v>
       </c>
       <c r="F54" t="n">
-        <v>1631236299</v>
-      </c>
-      <c r="G54" t="b">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G54" t="n">
+        <v>21</v>
       </c>
       <c r="H54" t="n">
-        <v>1</v>
+        <v>-32.939457</v>
       </c>
       <c r="I54" t="n">
-        <v>9</v>
-      </c>
-      <c r="J54" t="n">
-        <v>11</v>
-      </c>
-      <c r="K54" t="n">
-        <v>-32.939457</v>
-      </c>
-      <c r="L54" t="n">
         <v>-60.679149</v>
       </c>
     </row>
@@ -2844,30 +2246,19 @@
       <c r="D55" t="n">
         <v>54</v>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E55" t="n">
+        <v>5</v>
       </c>
       <c r="F55" t="n">
-        <v>1631236288</v>
-      </c>
-      <c r="G55" t="b">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="G55" t="n">
+        <v>21</v>
       </c>
       <c r="H55" t="n">
-        <v>1</v>
+        <v>-32.9581866</v>
       </c>
       <c r="I55" t="n">
-        <v>8</v>
-      </c>
-      <c r="J55" t="n">
-        <v>11</v>
-      </c>
-      <c r="K55" t="n">
-        <v>-32.9581866</v>
-      </c>
-      <c r="L55" t="n">
         <v>-60.6913242</v>
       </c>
     </row>
@@ -2888,30 +2279,19 @@
       <c r="D56" t="n">
         <v>56</v>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E56" t="n">
+        <v>7</v>
       </c>
       <c r="F56" t="n">
-        <v>1631236299</v>
-      </c>
-      <c r="G56" t="b">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="G56" t="n">
+        <v>19</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>-32.9093257</v>
       </c>
       <c r="I56" t="n">
-        <v>13</v>
-      </c>
-      <c r="J56" t="n">
-        <v>6</v>
-      </c>
-      <c r="K56" t="n">
-        <v>-32.9093257</v>
-      </c>
-      <c r="L56" t="n">
         <v>-60.6833951</v>
       </c>
     </row>
@@ -2932,30 +2312,19 @@
       <c r="D57" t="n">
         <v>57</v>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E57" t="n">
+        <v>15</v>
       </c>
       <c r="F57" t="n">
-        <v>1631236291</v>
-      </c>
-      <c r="G57" t="b">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G57" t="n">
+        <v>21</v>
       </c>
       <c r="H57" t="n">
-        <v>0</v>
+        <v>-32.91422795893311</v>
       </c>
       <c r="I57" t="n">
-        <v>8</v>
-      </c>
-      <c r="J57" t="n">
-        <v>12</v>
-      </c>
-      <c r="K57" t="n">
-        <v>-32.91422795893311</v>
-      </c>
-      <c r="L57" t="n">
         <v>-60.68635056866098</v>
       </c>
     </row>
@@ -2976,30 +2345,19 @@
       <c r="D58" t="n">
         <v>60</v>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E58" t="n">
+        <v>8</v>
       </c>
       <c r="F58" t="n">
-        <v>1631236274</v>
-      </c>
-      <c r="G58" t="b">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="G58" t="n">
+        <v>21</v>
       </c>
       <c r="H58" t="n">
-        <v>0</v>
+        <v>-32.89464556057717</v>
       </c>
       <c r="I58" t="n">
-        <v>6</v>
-      </c>
-      <c r="J58" t="n">
-        <v>14</v>
-      </c>
-      <c r="K58" t="n">
-        <v>-32.89464556057717</v>
-      </c>
-      <c r="L58" t="n">
         <v>-60.69265425549448</v>
       </c>
     </row>
@@ -3020,30 +2378,19 @@
       <c r="D59" t="n">
         <v>59</v>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E59" t="n">
+        <v>6</v>
       </c>
       <c r="F59" t="n">
-        <v>1631236280</v>
-      </c>
-      <c r="G59" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G59" t="n">
+        <v>15</v>
       </c>
       <c r="H59" t="n">
-        <v>0</v>
+        <v>-32.9004262817609</v>
       </c>
       <c r="I59" t="n">
-        <v>8</v>
-      </c>
-      <c r="J59" t="n">
-        <v>7</v>
-      </c>
-      <c r="K59" t="n">
-        <v>-32.9004262817609</v>
-      </c>
-      <c r="L59" t="n">
         <v>-60.69081468532575</v>
       </c>
     </row>
@@ -3064,30 +2411,19 @@
       <c r="D60" t="n">
         <v>55</v>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E60" t="n">
+        <v>7</v>
       </c>
       <c r="F60" t="n">
-        <v>1631236299</v>
-      </c>
-      <c r="G60" t="b">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="G60" t="n">
+        <v>19</v>
       </c>
       <c r="H60" t="n">
-        <v>1</v>
+        <v>-32.91293717782394</v>
       </c>
       <c r="I60" t="n">
-        <v>12</v>
-      </c>
-      <c r="J60" t="n">
-        <v>8</v>
-      </c>
-      <c r="K60" t="n">
-        <v>-32.91293717782394</v>
-      </c>
-      <c r="L60" t="n">
         <v>-60.68009608761775</v>
       </c>
     </row>
@@ -3108,30 +2444,19 @@
       <c r="D61" t="n">
         <v>61</v>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E61" t="n">
+        <v>32</v>
       </c>
       <c r="F61" t="n">
-        <v>1631236292</v>
-      </c>
-      <c r="G61" t="b">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="G61" t="n">
+        <v>44</v>
       </c>
       <c r="H61" t="n">
-        <v>1</v>
+        <v>-32.89180515414552</v>
       </c>
       <c r="I61" t="n">
-        <v>26</v>
-      </c>
-      <c r="J61" t="n">
-        <v>15</v>
-      </c>
-      <c r="K61" t="n">
-        <v>-32.89180515414552</v>
-      </c>
-      <c r="L61" t="n">
         <v>-60.68577111042986</v>
       </c>
     </row>
@@ -3152,30 +2477,19 @@
       <c r="D62" t="n">
         <v>62</v>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E62" t="n">
+        <v>14</v>
       </c>
       <c r="F62" t="n">
-        <v>1631236304</v>
-      </c>
-      <c r="G62" t="b">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G62" t="n">
+        <v>20</v>
       </c>
       <c r="H62" t="n">
-        <v>0</v>
+        <v>-32.88490773761225</v>
       </c>
       <c r="I62" t="n">
-        <v>5</v>
-      </c>
-      <c r="J62" t="n">
-        <v>15</v>
-      </c>
-      <c r="K62" t="n">
-        <v>-32.88490773761225</v>
-      </c>
-      <c r="L62" t="n">
         <v>-60.68735302130975</v>
       </c>
     </row>
@@ -3196,30 +2510,19 @@
       <c r="D63" t="n">
         <v>63</v>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E63" t="n">
+        <v>12</v>
       </c>
       <c r="F63" t="n">
-        <v>1631236304</v>
-      </c>
-      <c r="G63" t="b">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="G63" t="n">
+        <v>19</v>
       </c>
       <c r="H63" t="n">
-        <v>0</v>
+        <v>-32.910503</v>
       </c>
       <c r="I63" t="n">
-        <v>14</v>
-      </c>
-      <c r="J63" t="n">
-        <v>6</v>
-      </c>
-      <c r="K63" t="n">
-        <v>-32.910503</v>
-      </c>
-      <c r="L63" t="n">
         <v>-60.677572</v>
       </c>
     </row>
@@ -3240,30 +2543,19 @@
       <c r="D64" t="n">
         <v>58</v>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E64" t="n">
+        <v>12</v>
       </c>
       <c r="F64" t="n">
-        <v>1631236283</v>
-      </c>
-      <c r="G64" t="b">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="G64" t="n">
+        <v>17</v>
       </c>
       <c r="H64" t="n">
-        <v>0</v>
+        <v>-32.90654927658849</v>
       </c>
       <c r="I64" t="n">
-        <v>14</v>
-      </c>
-      <c r="J64" t="n">
-        <v>2</v>
-      </c>
-      <c r="K64" t="n">
-        <v>-32.90654927658849</v>
-      </c>
-      <c r="L64" t="n">
         <v>-60.6889224677472</v>
       </c>
     </row>
@@ -3284,30 +2576,19 @@
       <c r="D65" t="n">
         <v>64</v>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E65" t="n">
+        <v>14</v>
       </c>
       <c r="F65" t="n">
-        <v>1631236274</v>
-      </c>
-      <c r="G65" t="b">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="G65" t="n">
+        <v>21</v>
       </c>
       <c r="H65" t="n">
-        <v>0</v>
+        <v>-32.942375</v>
       </c>
       <c r="I65" t="n">
-        <v>11</v>
-      </c>
-      <c r="J65" t="n">
-        <v>9</v>
-      </c>
-      <c r="K65" t="n">
-        <v>-32.942375</v>
-      </c>
-      <c r="L65" t="n">
         <v>-60.691032</v>
       </c>
     </row>
@@ -3328,30 +2609,19 @@
       <c r="D66" t="n">
         <v>65</v>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E66" t="n">
+        <v>13</v>
       </c>
       <c r="F66" t="n">
-        <v>1631236298</v>
-      </c>
-      <c r="G66" t="b">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="G66" t="n">
+        <v>21</v>
       </c>
       <c r="H66" t="n">
-        <v>3</v>
+        <v>-32.941427</v>
       </c>
       <c r="I66" t="n">
-        <v>6</v>
-      </c>
-      <c r="J66" t="n">
-        <v>14</v>
-      </c>
-      <c r="K66" t="n">
-        <v>-32.941427</v>
-      </c>
-      <c r="L66" t="n">
         <v>-60.696252</v>
       </c>
     </row>
@@ -3372,30 +2642,19 @@
       <c r="D67" t="n">
         <v>66</v>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E67" t="n">
+        <v>11</v>
       </c>
       <c r="F67" t="n">
-        <v>1631236278</v>
-      </c>
-      <c r="G67" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G67" t="n">
+        <v>20</v>
       </c>
       <c r="H67" t="n">
-        <v>2</v>
+        <v>-32.940079</v>
       </c>
       <c r="I67" t="n">
-        <v>9</v>
-      </c>
-      <c r="J67" t="n">
-        <v>11</v>
-      </c>
-      <c r="K67" t="n">
-        <v>-32.940079</v>
-      </c>
-      <c r="L67" t="n">
         <v>-60.705073</v>
       </c>
     </row>
@@ -3416,30 +2675,19 @@
       <c r="D68" t="n">
         <v>67</v>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E68" t="n">
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>1631236284</v>
-      </c>
-      <c r="G68" t="b">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="G68" t="n">
+        <v>21</v>
       </c>
       <c r="H68" t="n">
-        <v>1</v>
+        <v>-32.940247</v>
       </c>
       <c r="I68" t="n">
-        <v>14</v>
-      </c>
-      <c r="J68" t="n">
-        <v>6</v>
-      </c>
-      <c r="K68" t="n">
-        <v>-32.940247</v>
-      </c>
-      <c r="L68" t="n">
         <v>-60.711147</v>
       </c>
     </row>
@@ -3460,30 +2708,19 @@
       <c r="D69" t="n">
         <v>68</v>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E69" t="n">
+        <v>7</v>
       </c>
       <c r="F69" t="n">
-        <v>1631236279</v>
-      </c>
-      <c r="G69" t="b">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="G69" t="n">
+        <v>20</v>
       </c>
       <c r="H69" t="n">
-        <v>0</v>
+        <v>-32.933226</v>
       </c>
       <c r="I69" t="n">
-        <v>10</v>
-      </c>
-      <c r="J69" t="n">
-        <v>9</v>
-      </c>
-      <c r="K69" t="n">
-        <v>-32.933226</v>
-      </c>
-      <c r="L69" t="n">
         <v>-60.713076</v>
       </c>
     </row>
@@ -3504,30 +2741,19 @@
       <c r="D70" t="n">
         <v>69</v>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E70" t="n">
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>1631236294</v>
-      </c>
-      <c r="G70" t="b">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="G70" t="n">
+        <v>20</v>
       </c>
       <c r="H70" t="n">
-        <v>0</v>
+        <v>-32.928205</v>
       </c>
       <c r="I70" t="n">
-        <v>11</v>
-      </c>
-      <c r="J70" t="n">
-        <v>9</v>
-      </c>
-      <c r="K70" t="n">
-        <v>-32.928205</v>
-      </c>
-      <c r="L70" t="n">
         <v>-60.712881</v>
       </c>
     </row>
@@ -3548,30 +2774,19 @@
       <c r="D71" t="n">
         <v>70</v>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E71" t="n">
+        <v>12</v>
       </c>
       <c r="F71" t="n">
-        <v>1631236302</v>
-      </c>
-      <c r="G71" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G71" t="n">
+        <v>21</v>
       </c>
       <c r="H71" t="n">
-        <v>0</v>
+        <v>-32.884702</v>
       </c>
       <c r="I71" t="n">
-        <v>9</v>
-      </c>
-      <c r="J71" t="n">
-        <v>11</v>
-      </c>
-      <c r="K71" t="n">
-        <v>-32.884702</v>
-      </c>
-      <c r="L71" t="n">
         <v>-60.695824</v>
       </c>
     </row>
@@ -3592,30 +2807,19 @@
       <c r="D72" t="n">
         <v>71</v>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E72" t="n">
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>1631236277</v>
-      </c>
-      <c r="G72" t="b">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="G72" t="n">
+        <v>22</v>
       </c>
       <c r="H72" t="n">
-        <v>1</v>
+        <v>-32.878274</v>
       </c>
       <c r="I72" t="n">
-        <v>10</v>
-      </c>
-      <c r="J72" t="n">
-        <v>10</v>
-      </c>
-      <c r="K72" t="n">
-        <v>-32.878274</v>
-      </c>
-      <c r="L72" t="n">
         <v>-60.697782</v>
       </c>
     </row>
@@ -3636,30 +2840,19 @@
       <c r="D73" t="n">
         <v>72</v>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
+      <c r="E73" t="n">
+        <v>14</v>
       </c>
       <c r="F73" t="n">
-        <v>1631236278</v>
-      </c>
-      <c r="G73" t="b">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="G73" t="n">
+        <v>21</v>
       </c>
       <c r="H73" t="n">
-        <v>0</v>
+        <v>-32.8736414</v>
       </c>
       <c r="I73" t="n">
-        <v>13</v>
-      </c>
-      <c r="J73" t="n">
-        <v>7</v>
-      </c>
-      <c r="K73" t="n">
-        <v>-32.8736414</v>
-      </c>
-      <c r="L73" t="n">
         <v>-60.6890764</v>
       </c>
     </row>

</xml_diff>